<commit_message>
Refactor: make excel reader use the common column parsers, and delete the ones previously in the excel reader module
</commit_message>
<xml_diff>
--- a/tables/readers/tests/input/foo.xlsx
+++ b/tables/readers/tests/input/foo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeaco\repos\pdtable\tables\readers\tests\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A5EF5A-3D28-4207-AD66-85A89AFBE92E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7E0D3F-3E84-4E2C-ACB2-4691C3BB5B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="3315" windowWidth="23040" windowHeight="11970" xr2:uid="{0C2B564F-1ED4-41D9-860E-6D5D2FB64FA7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{0C2B564F-1ED4-41D9-860E-6D5D2FB64FA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>all</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>FaLsE</t>
   </si>
 </sst>
 </file>
@@ -122,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,22 +445,22 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -467,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -478,7 +482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -489,7 +493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -500,39 +504,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -540,7 +544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -548,7 +552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -556,7 +560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -564,7 +568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>42</v>
       </c>

</xml_diff>